<commit_message>
Update Practice.xls and upload source code
</commit_message>
<xml_diff>
--- a/Olympic-2014/Practices.xlsx
+++ b/Olympic-2014/Practices.xlsx
@@ -889,10 +889,10 @@
   <dimension ref="A1:W50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B26" sqref="B26"/>
+      <selection pane="bottomRight" activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1862,10 +1862,14 @@
       </c>
       <c r="D20" s="12">
         <f t="shared" si="0"/>
-        <v>4.5</v>
-      </c>
-      <c r="E20" s="8"/>
-      <c r="F20" s="9"/>
+        <v>4.2</v>
+      </c>
+      <c r="E20" s="8">
+        <v>3</v>
+      </c>
+      <c r="F20" s="9">
+        <v>100</v>
+      </c>
       <c r="G20" s="5"/>
       <c r="H20" s="8"/>
       <c r="I20" s="9"/>
@@ -1905,7 +1909,6 @@
         <v>3.8</v>
       </c>
       <c r="E21" s="8"/>
-      <c r="F21" s="9"/>
       <c r="G21" s="5"/>
       <c r="H21" s="8"/>
       <c r="I21" s="9"/>
@@ -2108,10 +2111,14 @@
       </c>
       <c r="D26" s="12">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E26" s="8"/>
-      <c r="F26" s="9"/>
+        <v>3.8</v>
+      </c>
+      <c r="E26" s="8">
+        <v>3</v>
+      </c>
+      <c r="F26" s="9">
+        <v>100</v>
+      </c>
       <c r="G26" s="5"/>
       <c r="H26" s="8"/>
       <c r="I26" s="9"/>

</xml_diff>